<commit_message>
Fix missing policy ID number in WebAppData for Ban New Power Plants[lignite es]
</commit_message>
<xml_diff>
--- a/WebAppData.xlsx
+++ b/WebAppData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-mexico\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15BE394-B3C0-484B-93C3-70A2C9451CFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="465" windowWidth="19425" windowHeight="11025"/>
+    <workbookView xWindow="2490" yWindow="1020" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="10" r:id="rId1"/>
@@ -18,17 +24,27 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PolicyLevers!$A$1:$U$326</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Jeffrey Rissman</author>
   </authors>
   <commentList>
-    <comment ref="K140" authorId="0">
+    <comment ref="K140" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K142" authorId="0">
+    <comment ref="K142" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,11 +97,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="OuputGraphSchema" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="OuputGraphSchema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="Z:\todd\Projects\PolicySolutions\tools\lib\OuputGraphSchema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
-  <connection id="2" name="PolicyLeverSchema" type="4" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="PolicyLeverSchema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="Z:\todd\Projects\PolicySolutions\tools\lib\PolicyLeverSchema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -4048,7 +4064,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
@@ -5023,28 +5039,28 @@
     </xf>
   </cellXfs>
   <cellStyles count="22">
-    <cellStyle name="2x indented GHG Textfiels" xfId="10"/>
-    <cellStyle name="5x indented GHG Textfiels" xfId="11"/>
-    <cellStyle name="AggCels" xfId="12"/>
-    <cellStyle name="AggGreen_bld" xfId="15"/>
-    <cellStyle name="Body: normal cell 2" xfId="5"/>
-    <cellStyle name="Comma 2" xfId="21"/>
-    <cellStyle name="Comma 6" xfId="6"/>
-    <cellStyle name="Constants" xfId="8"/>
-    <cellStyle name="CustomizationCells" xfId="17"/>
-    <cellStyle name="Empty_B_border" xfId="16"/>
-    <cellStyle name="Header: bottom row 2" xfId="4"/>
-    <cellStyle name="Headline" xfId="7"/>
+    <cellStyle name="2x indented GHG Textfiels" xfId="10" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="5x indented GHG Textfiels" xfId="11" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="AggCels" xfId="12" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="AggGreen_bld" xfId="15" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Body: normal cell 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 6" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Constants" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="CustomizationCells" xfId="17" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Empty_B_border" xfId="16" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Header: bottom row 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Headline" xfId="7" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="18"/>
-    <cellStyle name="Normal 4" xfId="19"/>
-    <cellStyle name="Normal GHG Textfiels Bold" xfId="9"/>
-    <cellStyle name="Normal GHG-Shade" xfId="14"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 3" xfId="18" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 4" xfId="19" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal GHG Textfiels Bold" xfId="9" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal GHG-Shade" xfId="14" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="20"/>
-    <cellStyle name="Обычный_CRF2002 (1)" xfId="13"/>
+    <cellStyle name="Percent 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Обычный_CRF2002 (1)" xfId="13" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
@@ -5250,7 +5266,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5311,7 +5327,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5372,7 +5388,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5433,7 +5449,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5748,7 +5764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5824,12 +5840,12 @@
     <row r="24" spans="1:1">
       <c r="A24" s="10">
         <f>MAX(PolicyLevers!H:H)</f>
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A10" r:id="rId1"/>
+    <hyperlink ref="A10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -5837,12 +5853,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U333"/>
   <sheetViews>
-    <sheetView topLeftCell="A200" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B206" sqref="B206:J207"/>
-    </sheetView>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -12799,7 +12813,9 @@
         <v>562</v>
       </c>
       <c r="G120" s="56"/>
-      <c r="H120" s="57"/>
+      <c r="H120" s="57">
+        <v>206</v>
+      </c>
       <c r="I120" s="56" t="s">
         <v>54</v>
       </c>
@@ -24221,7 +24237,7 @@
       <c r="I333" s="53"/>
     </row>
   </sheetData>
-  <sortState ref="A119:I139">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A119:I139">
     <sortCondition ref="B119:B139"/>
   </sortState>
   <conditionalFormatting sqref="I1 I21:I33 I35:I39 I43 I51 I57 I63 I279:I309 I311 I313:I332 I334:I1048576 I66:I205 I208:I277">
@@ -24310,7 +24326,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="T212" r:id="rId1" display="https://www.fas.org/sgp/crs/misc/R40562.pdf, p.3, paragraph 1"/>
+    <hyperlink ref="T212" r:id="rId1" display="https://www.fas.org/sgp/crs/misc/R40562.pdf, p.3, paragraph 1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
@@ -24322,7 +24338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26273,7 +26289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26324,7 +26340,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E94"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -27050,9 +27066,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1"/>
-    <hyperlink ref="A63" r:id="rId2"/>
-    <hyperlink ref="A69" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A63" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="A69" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -27060,7 +27076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AM197"/>
   <sheetViews>
     <sheetView topLeftCell="A153" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
@@ -28527,7 +28543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S100"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>